<commit_message>
write amd read XL new features release
</commit_message>
<xml_diff>
--- a/sw-tree-manager_Template.xlsx
+++ b/sw-tree-manager_Template.xlsx
@@ -1,40 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Programs\Macros\SW TreeManager\SW TreeManager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8872002F-9BF7-4D92-8981-C2D38612ED35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F39434F-F649-4DB5-B9C6-019841B9C1F9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3B5A501E-177A-4640-9997-B0183F223BA1}"/>
+    <workbookView xWindow="3810" yWindow="3810" windowWidth="21600" windowHeight="11385" xr2:uid="{3B5A501E-177A-4640-9997-B0183F223BA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Item No</t>
   </si>
@@ -49,9 +40,6 @@
   </si>
   <si>
     <t>Material</t>
-  </si>
-  <si>
-    <t>Drawing No</t>
   </si>
 </sst>
 </file>
@@ -414,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D9B61B8-2045-485B-867E-DA25E08A90AA}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +416,7 @@
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,9 +432,6 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>